<commit_message>
added comparison code and results
</commit_message>
<xml_diff>
--- a/test_speeches/predictions/Coding_Differneces_103_AI.xlsx
+++ b/test_speeches/predictions/Coding_Differneces_103_AI.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Metaphor/Similie</t>
+          <t>Metaphor/Simile</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -456,7 +456,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Stories/Anecdotes</t>
+          <t>Stories / anecdotes</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -466,27 +466,27 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Lists</t>
+          <t xml:space="preserve">Lists / Repetition </t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Repetition</t>
+          <t>Moral conviction</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Moral_conviction</t>
+          <t>Sentiment of the collective</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Sentiment_of_the_collective</t>
+          <t>Ambitious goals / Setting high expectations</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Setting_high_expectations</t>
+          <t>Confidence in goals</t>
         </is>
       </c>
     </row>

</xml_diff>